<commit_message>
added tests & fixes
</commit_message>
<xml_diff>
--- a/documentation/src/burndown-chart.xlsx
+++ b/documentation/src/burndown-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\withdrive\documentation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31325D37-B629-4569-8DC8-0FB2A55ABBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D95F843-E24C-4161-8C4A-E85A24465F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8DE94FC4-89CF-4120-BF4E-C3A5A20C23A8}"/>
   </bookViews>
@@ -305,7 +305,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Withdrive Sprint 4 Burndown chart</a:t>
+              <a:t>Withdrive Sprint 5 Burndown chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -461,61 +461,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>29.45</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.9</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.7</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.149999999999999</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.600000000000001</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.049999999999997</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.95</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.399999999999999</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.849999999999998</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.75</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.6499999999999986</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.0999999999999979</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5500000000000007</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -646,28 +646,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>20</c:v>
@@ -676,31 +676,31 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1817,7 +1817,7 @@
   <dimension ref="D5:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,10 +1860,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="7">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F9" s="7">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.25">
@@ -1872,10 +1872,10 @@
       </c>
       <c r="E10" s="7">
         <f>$E$9-D10*($E$9/$D$29)</f>
-        <v>29.45</v>
+        <v>38</v>
       </c>
       <c r="F10" s="7">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.25">
@@ -1884,10 +1884,10 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ref="E11:E29" si="0">$E$9-D11*($E$9/$D$29)</f>
-        <v>27.9</v>
+        <v>36</v>
       </c>
       <c r="F11" s="7">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.25">
@@ -1896,10 +1896,10 @@
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>26.35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="7">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.25">
@@ -1908,10 +1908,10 @@
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>24.8</v>
+        <v>32</v>
       </c>
       <c r="F13" s="7">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.25">
@@ -1920,10 +1920,10 @@
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>23.25</v>
+        <v>30</v>
       </c>
       <c r="F14" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.25">
@@ -1932,10 +1932,10 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>21.7</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.25">
@@ -1944,10 +1944,10 @@
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>20.149999999999999</v>
+        <v>26</v>
       </c>
       <c r="F16" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
@@ -1956,10 +1956,10 @@
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>18.600000000000001</v>
+        <v>24</v>
       </c>
       <c r="F17" s="7">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>17.049999999999997</v>
+        <v>22</v>
       </c>
       <c r="F18" s="7">
         <v>20</v>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
-        <v>15.5</v>
+        <v>20</v>
       </c>
       <c r="F19" s="7">
         <v>20</v>
@@ -1992,10 +1992,10 @@
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>13.95</v>
+        <v>18</v>
       </c>
       <c r="F20" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -2004,10 +2004,10 @@
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
-        <v>12.399999999999999</v>
+        <v>16</v>
       </c>
       <c r="F21" s="7">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
@@ -2016,10 +2016,10 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>10.849999999999998</v>
+        <v>14</v>
       </c>
       <c r="F22" s="7">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
@@ -2028,10 +2028,10 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>9.3000000000000007</v>
+        <v>12</v>
       </c>
       <c r="F23" s="7">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
@@ -2040,10 +2040,10 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>7.75</v>
+        <v>10</v>
       </c>
       <c r="F24" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
@@ -2052,10 +2052,10 @@
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
-        <v>6.1999999999999993</v>
+        <v>8</v>
       </c>
       <c r="F25" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
@@ -2064,10 +2064,10 @@
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
-        <v>4.6499999999999986</v>
+        <v>6</v>
       </c>
       <c r="F26" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="E27" s="7">
         <f t="shared" si="0"/>
-        <v>3.0999999999999979</v>
+        <v>4</v>
       </c>
       <c r="F27" s="7">
         <v>5</v>
@@ -2088,10 +2088,10 @@
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>1.5500000000000007</v>
+        <v>2</v>
       </c>
       <c r="F28" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final changes for submission sprint 5
</commit_message>
<xml_diff>
--- a/documentation/src/burndown-chart.xlsx
+++ b/documentation/src/burndown-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\withdrive\documentation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D95F843-E24C-4161-8C4A-E85A24465F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFBE4DD-5BED-4E00-81A6-6E86C100159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8DE94FC4-89CF-4120-BF4E-C3A5A20C23A8}"/>
   </bookViews>
@@ -676,16 +676,16 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>20</c:v>
@@ -1817,7 +1817,7 @@
   <dimension ref="D5:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,7 +1995,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -2007,7 +2007,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final sprint 6 changes
</commit_message>
<xml_diff>
--- a/documentation/src/burndown-chart.xlsx
+++ b/documentation/src/burndown-chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\withdrive\documentation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFBE4DD-5BED-4E00-81A6-6E86C100159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9306B39-0907-4788-BC93-6C4C5D32758E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8DE94FC4-89CF-4120-BF4E-C3A5A20C23A8}"/>
   </bookViews>
@@ -305,7 +305,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Withdrive Sprint 5 Burndown chart</a:t>
+              <a:t>Withdrive Sprint 6 Burndown chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -461,61 +461,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>21.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>8.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -646,61 +646,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1817,7 +1817,7 @@
   <dimension ref="D5:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,10 +1860,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.25">
@@ -1872,10 +1872,10 @@
       </c>
       <c r="E10" s="7">
         <f>$E$9-D10*($E$9/$D$29)</f>
-        <v>38</v>
+        <v>23.75</v>
       </c>
       <c r="F10" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.25">
@@ -1884,10 +1884,10 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ref="E11:E29" si="0">$E$9-D11*($E$9/$D$29)</f>
-        <v>36</v>
+        <v>22.5</v>
       </c>
       <c r="F11" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.25">
@@ -1896,10 +1896,10 @@
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>21.25</v>
       </c>
       <c r="F12" s="7">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.25">
@@ -1908,10 +1908,10 @@
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.25">
@@ -1920,10 +1920,10 @@
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>18.75</v>
       </c>
       <c r="F14" s="7">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.25">
@@ -1932,10 +1932,10 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>17.5</v>
       </c>
       <c r="F15" s="7">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.25">
@@ -1944,10 +1944,10 @@
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>16.25</v>
       </c>
       <c r="F16" s="7">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
@@ -1956,10 +1956,10 @@
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F17" s="7">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
@@ -1968,10 +1968,10 @@
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>13.75</v>
       </c>
       <c r="F18" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
@@ -1980,10 +1980,10 @@
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>12.5</v>
       </c>
       <c r="F19" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
@@ -1992,10 +1992,10 @@
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>11.25</v>
       </c>
       <c r="F20" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -2004,10 +2004,10 @@
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F21" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
@@ -2016,10 +2016,10 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>8.75</v>
       </c>
       <c r="F22" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
@@ -2028,10 +2028,10 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="F23" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
@@ -2040,10 +2040,10 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6.25</v>
       </c>
       <c r="F24" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
@@ -2052,10 +2052,10 @@
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F25" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
@@ -2064,10 +2064,10 @@
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="F26" s="7">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="E27" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="F27" s="7">
         <v>5</v>
@@ -2088,10 +2088,10 @@
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="F28" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>